<commit_message>
se produce cada producto en un sector
</commit_message>
<xml_diff>
--- a/macro_sam_2008_analisis.xlsx
+++ b/macro_sam_2008_analisis.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11310"/>
   </bookViews>
   <sheets>
-    <sheet name="macro_sam_2008__simp" sheetId="9" r:id="rId1"/>
-    <sheet name="macro_sam_2008_simp0" sheetId="8" r:id="rId2"/>
+    <sheet name="macro_sam_2008__simp_1" sheetId="10" r:id="rId1"/>
+    <sheet name="macro_sam_2008__simp" sheetId="9" r:id="rId2"/>
     <sheet name="macro_sam_2008_v1" sheetId="7" r:id="rId3"/>
     <sheet name="macro_sam_2008" sheetId="1" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="192">
   <si>
     <t>Act prim</t>
   </si>
@@ -570,9 +570,6 @@
     <t>pasar los ingresos del capital y el trabajo row a los hogares</t>
   </si>
   <si>
-    <t>pasar SI row a los hogares</t>
-  </si>
-  <si>
     <t>Quitar del consumo de los hogares lo que se importa</t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>Se elimina el gasto intermedio en productos, el que se asigna al prod principal de cada actvidad y se cuadra la diferencia con hogares</t>
+  </si>
+  <si>
+    <t>Hacer que cada sector produzca un solo bien</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1102,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1115,7 +1115,6 @@
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="14" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1163,11 +1162,21 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1182,16 +1191,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1254,6 +1253,27 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1571,9 +1591,2188 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="12" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>14.341871281889999</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0</v>
+      </c>
+      <c r="T2" s="5">
+        <v>0</v>
+      </c>
+      <c r="U2" s="5">
+        <v>0</v>
+      </c>
+      <c r="V2" s="5">
+        <v>0</v>
+      </c>
+      <c r="W2" s="5">
+        <f>+SUM(B2:V2)</f>
+        <v>14.341871281889999</v>
+      </c>
+      <c r="X2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>19.770212353719991</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <f t="shared" ref="W3:W22" si="0">+SUM(B3:V3)</f>
+        <v>19.770212353719991</v>
+      </c>
+      <c r="X3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>49.380252786899987</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <f t="shared" si="0"/>
+        <v>49.380252786899987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>14.427016289780001</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1.75329745E-2</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0</v>
+      </c>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5">
+        <v>0.16482158305</v>
+      </c>
+      <c r="V5" s="12"/>
+      <c r="W5" s="5">
+        <f t="shared" si="0"/>
+        <v>14.60937084733</v>
+      </c>
+      <c r="Y5" s="7">
+        <f>+T5+J5</f>
+        <v>14.427016289780001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>4.1279825582999976</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>8.3720262130000001E-2</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5">
+        <v>20.612622200999997</v>
+      </c>
+      <c r="V6" s="12"/>
+      <c r="W6" s="5">
+        <f t="shared" si="0"/>
+        <v>24.824325021429996</v>
+      </c>
+      <c r="Y6" s="7">
+        <f t="shared" ref="Y6:Y7" si="1">+T6+J6</f>
+        <v>4.1279825582999976</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>37.466723587681663</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>10.39411222</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0</v>
+      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5">
+        <v>3.5847821083199998</v>
+      </c>
+      <c r="V7" s="12"/>
+      <c r="W7" s="5">
+        <f t="shared" si="0"/>
+        <v>51.445617916001666</v>
+      </c>
+      <c r="Y7" s="7">
+        <f t="shared" si="1"/>
+        <v>37.466723587681663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1.1501183518899984</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8.174254673719993</v>
+      </c>
+      <c r="D8" s="5">
+        <v>24.808658336899988</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
+        <v>0</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="0"/>
+        <v>34.133031362509982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>13.19175293</v>
+      </c>
+      <c r="C9" s="5">
+        <v>11.59595768</v>
+      </c>
+      <c r="D9" s="5">
+        <v>24.571594449999999</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0</v>
+      </c>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5">
+        <v>0</v>
+      </c>
+      <c r="V9" s="5">
+        <v>0</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="0"/>
+        <v>49.359305059999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>34.133031370000005</v>
+      </c>
+      <c r="I10" s="5">
+        <v>17.281502200000006</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>17.431284399999999</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0.55637803610000003</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>4.0619130575</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <f t="shared" si="0"/>
+        <v>73.464109063600006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>31.096709390000001</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>5.8570051300000001</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0</v>
+      </c>
+      <c r="T11" s="5">
+        <v>0</v>
+      </c>
+      <c r="U11" s="5">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5">
+        <f t="shared" si="0"/>
+        <v>36.953714519999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.98109349999999995</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1.6238783000000001</v>
+      </c>
+      <c r="N12" s="5">
+        <v>0</v>
+      </c>
+      <c r="O12" s="5">
+        <v>5.8828657</v>
+      </c>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="5">
+        <v>7.3869768860000002</v>
+      </c>
+      <c r="S12" s="12"/>
+      <c r="T12" s="5">
+        <v>0</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0</v>
+      </c>
+      <c r="V12" s="5">
+        <v>0</v>
+      </c>
+      <c r="W12" s="5">
+        <f t="shared" si="0"/>
+        <v>15.874814386000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>7.4808834299999996</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0</v>
+      </c>
+      <c r="U13" s="5">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0</v>
+      </c>
+      <c r="W13" s="5">
+        <f t="shared" si="0"/>
+        <v>7.4808834299999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>1.5233916200000002</v>
+      </c>
+      <c r="L14" s="5">
+        <v>2.5385214375</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0</v>
+      </c>
+      <c r="V14" s="5">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5">
+        <f t="shared" si="0"/>
+        <v>4.0619130575</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>1.2089669999999999</v>
+      </c>
+      <c r="K15" s="5">
+        <v>4.6738986999999996</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0</v>
+      </c>
+      <c r="S15" s="5">
+        <v>0</v>
+      </c>
+      <c r="T15" s="5">
+        <v>0</v>
+      </c>
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5">
+        <v>0</v>
+      </c>
+      <c r="W15" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8828657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0</v>
+      </c>
+      <c r="S16" s="5">
+        <v>0</v>
+      </c>
+      <c r="T16" s="5">
+        <v>0</v>
+      </c>
+      <c r="U16" s="5">
+        <v>0</v>
+      </c>
+      <c r="V16" s="5">
+        <v>0</v>
+      </c>
+      <c r="W16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5">
+        <v>0</v>
+      </c>
+      <c r="S17" s="5">
+        <v>0</v>
+      </c>
+      <c r="T17" s="5">
+        <v>0</v>
+      </c>
+      <c r="U17" s="5">
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <f>(254765.8734+B29)/1000000</f>
+        <v>0.26749955991000002</v>
+      </c>
+      <c r="F18" s="5">
+        <f>(5033784.004+C29)/1000000</f>
+        <v>5.0541126654799999</v>
+      </c>
+      <c r="G18" s="5">
+        <f>(578585.5105+D29)/1000000</f>
+        <v>2.0653646604999998</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+      <c r="R18" s="5">
+        <v>0</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0</v>
+      </c>
+      <c r="T18" s="5">
+        <v>0</v>
+      </c>
+      <c r="U18" s="5">
+        <v>0</v>
+      </c>
+      <c r="V18" s="5">
+        <v>0</v>
+      </c>
+      <c r="W18" s="5">
+        <f t="shared" si="0"/>
+        <v>7.3869768858900002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0</v>
+      </c>
+      <c r="O19" s="5">
+        <v>0</v>
+      </c>
+      <c r="P19" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>0</v>
+      </c>
+      <c r="R19" s="5">
+        <v>0</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0</v>
+      </c>
+      <c r="T19" s="5">
+        <v>0</v>
+      </c>
+      <c r="U19" s="5">
+        <v>0</v>
+      </c>
+      <c r="V19" s="5">
+        <v>0</v>
+      </c>
+      <c r="W19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5">
+        <v>0</v>
+      </c>
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>0</v>
+      </c>
+      <c r="R20" s="5">
+        <v>0</v>
+      </c>
+      <c r="S20" s="5">
+        <v>0</v>
+      </c>
+      <c r="T20" s="5">
+        <v>0</v>
+      </c>
+      <c r="U20" s="5">
+        <v>0</v>
+      </c>
+      <c r="V20" s="5">
+        <v>0</v>
+      </c>
+      <c r="W20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>8.7797730940000012</v>
+      </c>
+      <c r="K21" s="5">
+        <v>13.325139800000001</v>
+      </c>
+      <c r="L21" s="5">
+        <v>2.2573129999999999</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="5">
+        <v>0</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>0</v>
+      </c>
+      <c r="R21" s="5">
+        <v>0</v>
+      </c>
+      <c r="S21" s="5">
+        <v>0</v>
+      </c>
+      <c r="T21" s="12"/>
+      <c r="U21" s="5">
+        <v>0</v>
+      </c>
+      <c r="V21" s="5">
+        <v>0</v>
+      </c>
+      <c r="W21" s="5">
+        <f t="shared" si="0"/>
+        <v>24.362225894000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>0</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0</v>
+      </c>
+      <c r="P22" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>0</v>
+      </c>
+      <c r="R22" s="5">
+        <v>0</v>
+      </c>
+      <c r="S22" s="5">
+        <v>0</v>
+      </c>
+      <c r="T22" s="5">
+        <v>0</v>
+      </c>
+      <c r="U22" s="12"/>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5">
+        <f>+SUM(B2:B22)</f>
+        <v>14.341871281889999</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" ref="C23:V23" si="2">+SUM(C2:C22)</f>
+        <v>19.770212353719991</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="2"/>
+        <v>49.380252786899987</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="2"/>
+        <v>14.609370841799999</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>24.824325019199989</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="2"/>
+        <v>51.445617447399989</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="2"/>
+        <v>34.133031370000005</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="2"/>
+        <v>49.359305090000007</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="2"/>
+        <v>73.491345959761659</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="2"/>
+        <v>36.953714519999998</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="2"/>
+        <v>15.847577930230001</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="2"/>
+        <v>7.4808834300000004</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="2"/>
+        <v>4.0619130575</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="2"/>
+        <v>5.8828657</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="5">
+        <f t="shared" si="2"/>
+        <v>7.3869768860000002</v>
+      </c>
+      <c r="S23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="5">
+        <f t="shared" si="2"/>
+        <v>24.362225892369995</v>
+      </c>
+      <c r="V23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="B25">
+        <f t="array" ref="B25:V25">TRANSPOSE(W2:W22)</f>
+        <v>14.341871281889999</v>
+      </c>
+      <c r="C25">
+        <v>19.770212353719991</v>
+      </c>
+      <c r="D25">
+        <v>49.380252786899987</v>
+      </c>
+      <c r="E25">
+        <v>14.60937084733</v>
+      </c>
+      <c r="F25">
+        <v>24.824325021429996</v>
+      </c>
+      <c r="G25">
+        <v>51.445617916001666</v>
+      </c>
+      <c r="H25">
+        <v>34.133031362509982</v>
+      </c>
+      <c r="I25">
+        <v>49.359305059999997</v>
+      </c>
+      <c r="J25">
+        <v>73.464109063600006</v>
+      </c>
+      <c r="K25">
+        <v>36.953714519999998</v>
+      </c>
+      <c r="L25">
+        <v>15.874814386000001</v>
+      </c>
+      <c r="M25">
+        <v>7.4808834299999996</v>
+      </c>
+      <c r="N25">
+        <v>4.0619130575</v>
+      </c>
+      <c r="O25">
+        <v>5.8828657</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>7.3869768858900002</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>24.362225894000002</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="B27" s="2">
+        <f>ROUND(B23-B25,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ref="C27:V27" si="3">ROUND(C23-C25,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="5">
+        <v>12733.68651</v>
+      </c>
+      <c r="C29" s="5">
+        <v>20328.661479999999</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1486779.15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A31" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="N31" s="7">
+        <f>+N10-E48</f>
+        <v>4.0619130575</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="F32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="N32" s="7">
+        <f>+L14-E48</f>
+        <v>2.5385214375</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B34">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B46" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B48" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="5">
+        <v>3.1605375580000001</v>
+      </c>
+      <c r="C52" s="5">
+        <v>11.927984220000001</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.16408898730000002</v>
+      </c>
+      <c r="F52" s="7">
+        <f>+SUM(B52:D52)</f>
+        <v>15.2526107653</v>
+      </c>
+      <c r="H52" s="7">
+        <f>+F52-B56</f>
+        <v>0.73260728730000046</v>
+      </c>
+      <c r="J52" s="7">
+        <f>+J5+H52</f>
+        <v>15.159623577080001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" s="5">
+        <v>6.9137747879999996</v>
+      </c>
+      <c r="C53" s="5">
+        <v>22.11542081</v>
+      </c>
+      <c r="D53" s="5">
+        <v>11.39658985</v>
+      </c>
+      <c r="F53" s="7">
+        <f t="shared" ref="F53:F54" si="4">+SUM(B53:D53)</f>
+        <v>40.425785447999999</v>
+      </c>
+      <c r="H53" s="7">
+        <f>+F53-C56</f>
+        <v>-3.8729534620000052</v>
+      </c>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7">
+        <f t="shared" ref="J53:J54" si="5">+J6+H53</f>
+        <v>0.25502909629999237</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="5">
+        <v>4.4456911320000003</v>
+      </c>
+      <c r="C54" s="5">
+        <v>10.25533388</v>
+      </c>
+      <c r="D54" s="5">
+        <v>25.790391530000001</v>
+      </c>
+      <c r="F54" s="7">
+        <f t="shared" si="4"/>
+        <v>40.491416542000003</v>
+      </c>
+      <c r="H54" s="7">
+        <f>+F54-D56</f>
+        <v>3.1403461747000065</v>
+      </c>
+      <c r="J54" s="7">
+        <f t="shared" si="5"/>
+        <v>40.60706976238167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B56" s="7">
+        <f>+SUM(B52:B54)</f>
+        <v>14.520003478</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" ref="C56:D56" si="6">+SUM(C52:C54)</f>
+        <v>44.298738910000004</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="6"/>
+        <v>37.351070367299997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="5">
+        <v>14.16830558289</v>
+      </c>
+      <c r="C62" s="5">
+        <v>1.069724034</v>
+      </c>
+      <c r="D62" s="5">
+        <v>0.94155019620000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="5">
+        <v>0.17356569899999999</v>
+      </c>
+      <c r="C63" s="5">
+        <v>17.205046675719991</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1.318426093</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1.495441644</v>
+      </c>
+      <c r="D64" s="5">
+        <v>47.12027649769999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B66" s="7">
+        <f>+SUM(B62:B64)</f>
+        <v>14.341871281889999</v>
+      </c>
+      <c r="C66" s="7">
+        <f t="shared" ref="C66:D66" si="7">+SUM(C62:C64)</f>
+        <v>19.770212353719991</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="7"/>
+        <v>49.380252786899987</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B68" s="7">
+        <v>1.8377085351100018</v>
+      </c>
+      <c r="C68" s="7">
+        <v>-1.073173883719992</v>
+      </c>
+      <c r="D68" s="7">
+        <v>-0.76453463689998813</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="5">
+        <v>2.9878268870000002</v>
+      </c>
+      <c r="C69" s="5">
+        <v>7.1010807900000001</v>
+      </c>
+      <c r="D69" s="5">
+        <v>24.0441237</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B71" s="7">
+        <f>+B69-B68</f>
+        <v>1.1501183518899984</v>
+      </c>
+      <c r="C71" s="7">
+        <f t="shared" ref="C71:D71" si="8">+C69-C68</f>
+        <v>8.174254673719993</v>
+      </c>
+      <c r="D71" s="7">
+        <f t="shared" si="8"/>
+        <v>24.808658336899988</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B23:W23 W2:W22">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:V27">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:V22">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:D29">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B52:D54">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62:D64">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69:D69">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1884,9 +4083,9 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="5">
         <v>0</v>
       </c>
@@ -1936,7 +4135,7 @@
       <c r="U5" s="5">
         <v>0.16482158305</v>
       </c>
-      <c r="V5" s="13"/>
+      <c r="V5" s="12"/>
       <c r="W5" s="5">
         <f t="shared" si="0"/>
         <v>14.60937084733</v>
@@ -1950,9 +4149,9 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="5">
         <v>0</v>
       </c>
@@ -2002,7 +4201,7 @@
       <c r="U6" s="5">
         <v>20.612622200999997</v>
       </c>
-      <c r="V6" s="13"/>
+      <c r="V6" s="12"/>
       <c r="W6" s="5">
         <f t="shared" si="0"/>
         <v>24.824325021429996</v>
@@ -2016,9 +4215,9 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="5">
         <v>0</v>
       </c>
@@ -2068,7 +4267,7 @@
       <c r="U7" s="5">
         <v>3.5847821083199998</v>
       </c>
-      <c r="V7" s="13"/>
+      <c r="V7" s="12"/>
       <c r="W7" s="5">
         <f t="shared" si="0"/>
         <v>51.445617916001666</v>
@@ -2410,12 +4609,12 @@
       <c r="O12" s="5">
         <v>5.8828657</v>
       </c>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
       <c r="R12" s="5">
         <v>7.3869768860000002</v>
       </c>
-      <c r="S12" s="13"/>
+      <c r="S12" s="12"/>
       <c r="T12" s="5">
         <v>0</v>
       </c>
@@ -2650,9 +4849,9 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="5">
         <v>0</v>
       </c>
@@ -2719,7 +4918,7 @@
       <c r="B17" s="5">
         <v>0</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="5">
         <v>0</v>
       </c>
@@ -2870,9 +5069,9 @@
       <c r="D19" s="5">
         <v>0</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="5">
         <v>0</v>
       </c>
@@ -2936,11 +5135,11 @@
       <c r="D20" s="5">
         <v>0</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="5">
         <v>0</v>
       </c>
@@ -3043,7 +5242,7 @@
       <c r="S21" s="5">
         <v>0</v>
       </c>
-      <c r="T21" s="13"/>
+      <c r="T21" s="12"/>
       <c r="U21" s="5">
         <v>0</v>
       </c>
@@ -3116,7 +5315,7 @@
       <c r="T22" s="5">
         <v>0</v>
       </c>
-      <c r="U22" s="13"/>
+      <c r="U22" s="12"/>
       <c r="V22" s="5">
         <v>0</v>
       </c>
@@ -3428,42 +5627,42 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.15">
@@ -3575,1806 +5774,32 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B23:W23 W2:W22">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:V27">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:V22">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52:D54">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5">
-        <f>(28803039.28-B28)/1000000</f>
-        <v>28.79030559349</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1.069724034</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.94155019620000002</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0</v>
-      </c>
-      <c r="V2" s="5">
-        <f>+SUM(B2:U2)</f>
-        <v>30.801579823690002</v>
-      </c>
-      <c r="W2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.17356569899999999</v>
-      </c>
-      <c r="F3" s="5">
-        <f>(62723730.2-C28)/1000000</f>
-        <v>62.703401538519998</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1.318426093</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <f>+SUM(B3:U3)</f>
-        <v>64.195393330520005</v>
-      </c>
-      <c r="W3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1.495441644</v>
-      </c>
-      <c r="G4" s="5">
-        <f>(87052368.69-D28)/1000000</f>
-        <v>85.565589539999991</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
-        <f>+SUM(B4:U4)</f>
-        <v>87.061031183999987</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3.1605375580000001</v>
-      </c>
-      <c r="C5" s="5">
-        <v>11.927984220000001</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.16408898730000002</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>13.875543749</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>1.75329745E-2</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>0</v>
-      </c>
-      <c r="P5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="5">
-        <v>0</v>
-      </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="5">
-        <v>0.16482158305</v>
-      </c>
-      <c r="V5" s="5">
-        <f>+SUM(B5:U5)</f>
-        <v>29.310509071849999</v>
-      </c>
-      <c r="X5" s="7">
-        <f>+J5+T5</f>
-        <v>13.875543749</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5">
-        <v>6.9137747879999996</v>
-      </c>
-      <c r="C6" s="5">
-        <v>22.11542081</v>
-      </c>
-      <c r="D6" s="5">
-        <v>11.39658985</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>9.694142130000003</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>8.3720262130000001E-2</v>
-      </c>
-      <c r="M6" s="5">
-        <v>0</v>
-      </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="O6" s="5">
-        <v>0</v>
-      </c>
-      <c r="P6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>0</v>
-      </c>
-      <c r="R6" s="5">
-        <v>0</v>
-      </c>
-      <c r="S6" s="5">
-        <v>0</v>
-      </c>
-      <c r="T6" s="13"/>
-      <c r="U6" s="5">
-        <v>20.612622200999997</v>
-      </c>
-      <c r="V6" s="5">
-        <f>+SUM(B6:U6)</f>
-        <v>70.816270041129997</v>
-      </c>
-      <c r="X6" s="7">
-        <f t="shared" ref="X6:X7" si="0">+J6+T6</f>
-        <v>9.694142130000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5">
-        <v>4.4456911320000003</v>
-      </c>
-      <c r="C7" s="5">
-        <v>10.25533388</v>
-      </c>
-      <c r="D7" s="5">
-        <v>25.790391530000001</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>35.420655259</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>10.39411222</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
-        <v>0</v>
-      </c>
-      <c r="T7" s="13"/>
-      <c r="U7" s="5">
-        <v>3.5847821083199998</v>
-      </c>
-      <c r="V7" s="5">
-        <f>+SUM(B7:U7)</f>
-        <v>89.890966129319992</v>
-      </c>
-      <c r="X7" s="7">
-        <f t="shared" si="0"/>
-        <v>35.420655259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2.9878268870000002</v>
-      </c>
-      <c r="C8" s="5">
-        <v>7.1010807900000001</v>
-      </c>
-      <c r="D8" s="5">
-        <v>24.0441237</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5">
-        <v>0</v>
-      </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="O8" s="5">
-        <v>0</v>
-      </c>
-      <c r="P8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>0</v>
-      </c>
-      <c r="R8" s="5">
-        <v>0</v>
-      </c>
-      <c r="S8" s="5">
-        <v>0</v>
-      </c>
-      <c r="T8" s="5">
-        <v>0</v>
-      </c>
-      <c r="U8" s="5">
-        <v>0</v>
-      </c>
-      <c r="V8" s="5">
-        <f>+SUM(B8:U8)</f>
-        <v>34.133031377000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
-        <v>11.59595768</v>
-      </c>
-      <c r="D9" s="5">
-        <v>24.571594449999999</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="M9" s="5">
-        <v>0</v>
-      </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="O9" s="5">
-        <v>0</v>
-      </c>
-      <c r="P9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>0</v>
-      </c>
-      <c r="R9" s="5">
-        <v>0</v>
-      </c>
-      <c r="S9" s="5">
-        <v>0</v>
-      </c>
-      <c r="T9" s="12"/>
-      <c r="U9" s="5">
-        <v>0</v>
-      </c>
-      <c r="V9" s="5">
-        <f>+SUM(B9:U9)</f>
-        <v>40.167552129999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0</v>
-      </c>
-      <c r="C10" s="5">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="5">
-        <v>34.133031370000005</v>
-      </c>
-      <c r="I10" s="5">
-        <v>8.1355563510000035</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
-      <c r="K10" s="5">
-        <v>17.431284399999999</v>
-      </c>
-      <c r="L10" s="5">
-        <v>2.1073795340000001</v>
-      </c>
-      <c r="M10" s="5">
-        <v>0</v>
-      </c>
-      <c r="N10" s="5">
-        <v>5.5067667199999999</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-      <c r="P10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>0</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5">
-        <v>0</v>
-      </c>
-      <c r="T10" s="5">
-        <v>0</v>
-      </c>
-      <c r="U10" s="5">
-        <v>0</v>
-      </c>
-      <c r="V10" s="5">
-        <f>+SUM(B10:U10)</f>
-        <v>67.314018375000018</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0</v>
-      </c>
-      <c r="I11" s="5">
-        <v>31.096709390000001</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0</v>
-      </c>
-      <c r="L11" s="5">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5">
-        <v>5.8570051300000001</v>
-      </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="O11" s="5">
-        <v>0</v>
-      </c>
-      <c r="P11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>0</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0</v>
-      </c>
-      <c r="S11" s="5">
-        <v>0</v>
-      </c>
-      <c r="T11" s="5">
-        <v>0</v>
-      </c>
-      <c r="U11" s="5">
-        <v>0</v>
-      </c>
-      <c r="V11" s="5">
-        <f>+SUM(B11:U11)</f>
-        <v>36.953714519999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5">
-        <v>0</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.98109349999999995</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5">
-        <v>1.6238783000000001</v>
-      </c>
-      <c r="N12" s="5">
-        <v>0</v>
-      </c>
-      <c r="O12" s="5">
-        <v>5.8828657</v>
-      </c>
-      <c r="P12" s="5">
-        <v>1.444853663</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>0.95100149789999999</v>
-      </c>
-      <c r="R12" s="5">
-        <v>7.3869768860000002</v>
-      </c>
-      <c r="S12" s="5">
-        <v>0.5727635418</v>
-      </c>
-      <c r="T12" s="5">
-        <v>0</v>
-      </c>
-      <c r="U12" s="5">
-        <v>0</v>
-      </c>
-      <c r="V12" s="5">
-        <f>+SUM(B12:U12)</f>
-        <v>18.843433088699999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0</v>
-      </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>7.4808834299999996</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0</v>
-      </c>
-      <c r="L13" s="5">
-        <v>0</v>
-      </c>
-      <c r="M13" s="5">
-        <v>0</v>
-      </c>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
-      <c r="O13" s="5">
-        <v>0</v>
-      </c>
-      <c r="P13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>0</v>
-      </c>
-      <c r="R13" s="5">
-        <v>0</v>
-      </c>
-      <c r="S13" s="5">
-        <v>0</v>
-      </c>
-      <c r="T13" s="5">
-        <v>0</v>
-      </c>
-      <c r="U13" s="5">
-        <v>0</v>
-      </c>
-      <c r="V13" s="5">
-        <f>+SUM(B13:U13)</f>
-        <v>7.4808834299999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-      <c r="K14" s="5">
-        <v>1.5233916200000002</v>
-      </c>
-      <c r="L14" s="5">
-        <v>3.9833750999999999</v>
-      </c>
-      <c r="M14" s="5">
-        <v>0</v>
-      </c>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-      <c r="O14" s="5">
-        <v>0</v>
-      </c>
-      <c r="P14" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>0</v>
-      </c>
-      <c r="R14" s="5">
-        <v>0</v>
-      </c>
-      <c r="S14" s="5">
-        <v>0</v>
-      </c>
-      <c r="T14" s="5">
-        <v>0</v>
-      </c>
-      <c r="U14" s="5">
-        <v>0</v>
-      </c>
-      <c r="V14" s="5">
-        <f>+SUM(B14:U14)</f>
-        <v>5.5067667199999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1.2089669999999999</v>
-      </c>
-      <c r="K15" s="5">
-        <v>4.6738986999999996</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>0</v>
-      </c>
-      <c r="P15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
-        <v>0</v>
-      </c>
-      <c r="R15" s="5">
-        <v>0</v>
-      </c>
-      <c r="S15" s="5">
-        <v>0</v>
-      </c>
-      <c r="T15" s="5">
-        <v>0</v>
-      </c>
-      <c r="U15" s="5">
-        <v>0</v>
-      </c>
-      <c r="V15" s="5">
-        <f>+SUM(B15:U15)</f>
-        <v>5.8828657</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5">
-        <v>0.10199653260000001</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.2486144549</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1.0942426750000001</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5">
-        <v>0</v>
-      </c>
-      <c r="M16" s="5">
-        <v>0</v>
-      </c>
-      <c r="N16" s="5">
-        <v>0</v>
-      </c>
-      <c r="O16" s="5">
-        <v>0</v>
-      </c>
-      <c r="P16" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>0</v>
-      </c>
-      <c r="R16" s="5">
-        <v>0</v>
-      </c>
-      <c r="S16" s="5">
-        <v>0</v>
-      </c>
-      <c r="T16" s="5">
-        <v>0</v>
-      </c>
-      <c r="U16" s="5">
-        <v>0</v>
-      </c>
-      <c r="V16" s="5">
-        <f>+SUM(B16:U16)</f>
-        <v>1.4448536625000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0.95100149789999999</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>0</v>
-      </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5">
-        <v>0</v>
-      </c>
-      <c r="S17" s="5">
-        <v>0</v>
-      </c>
-      <c r="T17" s="5">
-        <v>0</v>
-      </c>
-      <c r="U17" s="5">
-        <v>0</v>
-      </c>
-      <c r="V17" s="5">
-        <f>+SUM(B17:U17)</f>
-        <v>0.95100149789999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <f>(254765.8734+B28)/1000000</f>
-        <v>0.26749955991000002</v>
-      </c>
-      <c r="F18" s="5">
-        <f>(5033784.004+C28)/1000000</f>
-        <v>5.0541126654799999</v>
-      </c>
-      <c r="G18" s="5">
-        <f>(578585.5105+D28)/1000000</f>
-        <v>2.0653646604999998</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5">
-        <v>0</v>
-      </c>
-      <c r="O18" s="5">
-        <v>0</v>
-      </c>
-      <c r="P18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="5">
-        <v>0</v>
-      </c>
-      <c r="R18" s="5">
-        <v>0</v>
-      </c>
-      <c r="S18" s="5">
-        <v>0</v>
-      </c>
-      <c r="T18" s="5">
-        <v>0</v>
-      </c>
-      <c r="U18" s="5">
-        <v>0</v>
-      </c>
-      <c r="V18" s="5">
-        <f>+SUM(B18:U18)</f>
-        <v>7.3869768858900002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5">
-        <v>0</v>
-      </c>
-      <c r="C19" s="5">
-        <v>0</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0</v>
-      </c>
-      <c r="E19" s="5">
-        <v>7.9138213919999992E-2</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0.49359015690000002</v>
-      </c>
-      <c r="G19" s="5">
-        <v>3.5171018349999999E-5</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
-        <v>0</v>
-      </c>
-      <c r="M19" s="5">
-        <v>0</v>
-      </c>
-      <c r="N19" s="5">
-        <v>0</v>
-      </c>
-      <c r="O19" s="5">
-        <v>0</v>
-      </c>
-      <c r="P19" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5">
-        <v>0</v>
-      </c>
-      <c r="R19" s="5">
-        <v>0</v>
-      </c>
-      <c r="S19" s="5">
-        <v>0</v>
-      </c>
-      <c r="T19" s="5">
-        <v>0</v>
-      </c>
-      <c r="U19" s="5">
-        <v>0</v>
-      </c>
-      <c r="V19" s="5">
-        <f>+SUM(B19:U19)</f>
-        <v>0.5727635418383501</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5">
-        <v>0</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>0</v>
-      </c>
-      <c r="L20" s="5">
-        <v>0</v>
-      </c>
-      <c r="M20" s="5">
-        <v>0</v>
-      </c>
-      <c r="N20" s="5">
-        <v>0</v>
-      </c>
-      <c r="O20" s="5">
-        <v>0</v>
-      </c>
-      <c r="P20" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="5">
-        <v>0</v>
-      </c>
-      <c r="R20" s="5">
-        <v>0</v>
-      </c>
-      <c r="S20" s="5">
-        <v>0</v>
-      </c>
-      <c r="T20" s="5">
-        <v>0</v>
-      </c>
-      <c r="U20" s="5">
-        <v>0</v>
-      </c>
-      <c r="V20" s="5">
-        <f>+SUM(B20:U20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
-        <v>0</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>8.7797730940000012</v>
-      </c>
-      <c r="K21" s="5">
-        <v>13.325139800000001</v>
-      </c>
-      <c r="L21" s="5">
-        <v>2.2573129999999999</v>
-      </c>
-      <c r="M21" s="5">
-        <v>0</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0</v>
-      </c>
-      <c r="P21" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>0</v>
-      </c>
-      <c r="R21" s="5">
-        <v>0</v>
-      </c>
-      <c r="S21" s="5">
-        <v>0</v>
-      </c>
-      <c r="T21" s="13"/>
-      <c r="U21" s="5">
-        <v>0</v>
-      </c>
-      <c r="V21" s="5">
-        <f>+SUM(B21:U21)</f>
-        <v>24.362225894000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="5">
-        <f>+SUM(B2:B21)</f>
-        <v>21.609826897600001</v>
-      </c>
-      <c r="C22" s="5">
-        <f>+SUM(C2:C21)</f>
-        <v>64.195393332799995</v>
-      </c>
-      <c r="D22" s="5">
-        <f>+SUM(D2:D21)</f>
-        <v>87.061031192299993</v>
-      </c>
-      <c r="E22" s="5">
-        <f>+SUM(E2:E21)</f>
-        <v>29.310509066320002</v>
-      </c>
-      <c r="F22" s="5">
-        <f>+SUM(F2:F21)</f>
-        <v>70.816270038900001</v>
-      </c>
-      <c r="G22" s="5">
-        <f>+SUM(G2:G21)</f>
-        <v>89.890965660718336</v>
-      </c>
-      <c r="H22" s="5">
-        <f>+SUM(H2:H21)</f>
-        <v>34.133031370000005</v>
-      </c>
-      <c r="I22" s="5">
-        <f>+SUM(I2:I21)</f>
-        <v>40.213359241000006</v>
-      </c>
-      <c r="J22" s="5">
-        <f>+SUM(J2:J21)</f>
-        <v>76.459964662000019</v>
-      </c>
-      <c r="K22" s="5">
-        <f>+SUM(K2:K21)</f>
-        <v>36.953714519999998</v>
-      </c>
-      <c r="L22" s="5">
-        <f>+SUM(L2:L21)</f>
-        <v>18.84343309063</v>
-      </c>
-      <c r="M22" s="5">
-        <f>+SUM(M2:M21)</f>
-        <v>7.4808834300000004</v>
-      </c>
-      <c r="N22" s="5">
-        <f>+SUM(N2:N21)</f>
-        <v>5.5067667199999999</v>
-      </c>
-      <c r="O22" s="5">
-        <f>+SUM(O2:O21)</f>
-        <v>5.8828657</v>
-      </c>
-      <c r="P22" s="5">
-        <f>+SUM(P2:P21)</f>
-        <v>1.444853663</v>
-      </c>
-      <c r="Q22" s="5">
-        <f>+SUM(Q2:Q21)</f>
-        <v>0.95100149789999999</v>
-      </c>
-      <c r="R22" s="5">
-        <f>+SUM(R2:R21)</f>
-        <v>7.3869768860000002</v>
-      </c>
-      <c r="S22" s="5">
-        <f>+SUM(S2:S21)</f>
-        <v>0.5727635418</v>
-      </c>
-      <c r="T22" s="5">
-        <f>+SUM(T2:T21)</f>
-        <v>0</v>
-      </c>
-      <c r="U22" s="5">
-        <f>+SUM(U2:U21)</f>
-        <v>24.362225892369995</v>
-      </c>
-      <c r="V22" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="B24">
-        <f t="array" ref="B24:U24">TRANSPOSE(V2:V21)</f>
-        <v>30.801579823690002</v>
-      </c>
-      <c r="C24">
-        <v>64.195393330520005</v>
-      </c>
-      <c r="D24">
-        <v>87.061031183999987</v>
-      </c>
-      <c r="E24">
-        <v>29.310509071849999</v>
-      </c>
-      <c r="F24">
-        <v>70.816270041129997</v>
-      </c>
-      <c r="G24">
-        <v>89.890966129319992</v>
-      </c>
-      <c r="H24">
-        <v>34.133031377000002</v>
-      </c>
-      <c r="I24">
-        <v>40.167552129999997</v>
-      </c>
-      <c r="J24">
-        <v>67.314018375000018</v>
-      </c>
-      <c r="K24">
-        <v>36.953714519999998</v>
-      </c>
-      <c r="L24">
-        <v>18.843433088699999</v>
-      </c>
-      <c r="M24">
-        <v>7.4808834299999996</v>
-      </c>
-      <c r="N24">
-        <v>5.5067667199999999</v>
-      </c>
-      <c r="O24">
-        <v>5.8828657</v>
-      </c>
-      <c r="P24">
-        <v>1.4448536625000001</v>
-      </c>
-      <c r="Q24">
-        <v>0.95100149789999999</v>
-      </c>
-      <c r="R24">
-        <v>7.3869768858900002</v>
-      </c>
-      <c r="S24">
-        <v>0.5727635418383501</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>24.362225894000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="B26" s="2">
-        <f>ROUND(B22-B24,1)</f>
-        <v>-9.1999999999999993</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" ref="C26:U26" si="1">ROUND(C22-C24,1)</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <f t="shared" si="1"/>
-        <v>9.1</v>
-      </c>
-      <c r="K26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="5">
-        <v>12733.68651</v>
-      </c>
-      <c r="C28" s="5">
-        <v>20328.661479999999</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1486779.15</v>
-      </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7">
-        <f>+J26+T26</f>
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="A30" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.15">
-      <c r="J31" s="7"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B34" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B35" t="s">
-        <v>182</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="V2:V21 B22:V22">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:U26">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U21">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28:D28">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7314,22 +7739,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B23:W23 W2:W22">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:V27">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:V22">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:D29">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10752,22 +11177,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:W23 W2:W22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:V27">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:V22">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
solo un producto y actividad
</commit_message>
<xml_diff>
--- a/macro_sam_2008_analisis.xlsx
+++ b/macro_sam_2008_analisis.xlsx
@@ -12,17 +12,18 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11310"/>
   </bookViews>
   <sheets>
-    <sheet name="macro_sam_2008__simp_1" sheetId="10" r:id="rId1"/>
-    <sheet name="macro_sam_2008__simp" sheetId="9" r:id="rId2"/>
-    <sheet name="macro_sam_2008_v1" sheetId="7" r:id="rId3"/>
-    <sheet name="macro_sam_2008" sheetId="1" r:id="rId4"/>
+    <sheet name="macro_sam_2008__simp_2" sheetId="11" r:id="rId1"/>
+    <sheet name="macro_sam_2008__simp_1" sheetId="10" r:id="rId2"/>
+    <sheet name="macro_sam_2008__simp" sheetId="9" r:id="rId3"/>
+    <sheet name="macro_sam_2008_v1" sheetId="7" r:id="rId4"/>
+    <sheet name="macro_sam_2008" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="195">
   <si>
     <t>Act prim</t>
   </si>
@@ -598,6 +599,15 @@
   </si>
   <si>
     <t>Hacer que cada sector produzca un solo bien</t>
+  </si>
+  <si>
+    <t>Act</t>
+  </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>Esta el la SAM que se está utilizando, con un solo producto producido en una sola actividad</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1172,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -1260,6 +1270,51 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1591,9 +1646,1036 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>83.492336422509979</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <f>+SUM(B2:M2)</f>
+        <v>83.492336422509979</v>
+      </c>
+      <c r="O2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="7">
+        <f>+SUM(C2:C2)</f>
+        <v>83.492336422509979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>56.02172243576166</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>10.495365456630001</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>24.362225892369995</v>
+      </c>
+      <c r="N3" s="5">
+        <f>+SUM(B3:M3)</f>
+        <v>90.879313784761649</v>
+      </c>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5">
+        <v>34.133031362509982</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <f>+SUM(B4:M4)</f>
+        <v>34.133031362509982</v>
+      </c>
+      <c r="Q4" s="7">
+        <f>+SUM(B4:B4)</f>
+        <v>34.133031362509982</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5">
+        <v>49.359305059999997</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <f>+SUM(B5:M5)</f>
+        <v>49.359305059999997</v>
+      </c>
+      <c r="Q5" s="7">
+        <f>+SUM(B5:B5)</f>
+        <v>49.359305059999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>34.133031370000005</v>
+      </c>
+      <c r="E6" s="5">
+        <v>17.281502200000006</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>17.431284399999999</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.55637803610000003</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>4.0619130575</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <f>+SUM(B6:M6)</f>
+        <v>73.464109063600006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>31.096709390000001</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5.8570051300000001</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <f>+SUM(B7:M7)</f>
+        <v>36.953714519999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.98109349999999995</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.6238783000000001</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
+        <v>5.8828657</v>
+      </c>
+      <c r="L8" s="5">
+        <v>7.3869768860000002</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <f>+SUM(B8:M8)</f>
+        <v>15.874814386000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>7.4808834299999996</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <f>+SUM(B9:M9)</f>
+        <v>7.4808834299999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1.5233916200000002</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2.5385214375</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <f>+SUM(B10:M10)</f>
+        <v>4.0619130575</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.2089669999999999</v>
+      </c>
+      <c r="G11" s="5">
+        <v>4.6738986999999996</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <f>+SUM(B11:M11)</f>
+        <v>5.8828657</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>7.3869768858900002</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
+        <f>+SUM(B12:M12)</f>
+        <v>7.3869768858900002</v>
+      </c>
+      <c r="Q12" s="7">
+        <f>+SUM(C12:C12)</f>
+        <v>7.3869768858900002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8.7797730940000012</v>
+      </c>
+      <c r="G13" s="5">
+        <v>13.325139800000001</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2.2573129999999999</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
+        <f>+SUM(B13:M13)</f>
+        <v>24.362225894000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="5">
+        <f>+SUM(B2:B13)</f>
+        <v>83.492336422509979</v>
+      </c>
+      <c r="C14" s="5">
+        <f>+SUM(C2:C13)</f>
+        <v>90.879313308399986</v>
+      </c>
+      <c r="D14" s="5">
+        <f>+SUM(D2:D13)</f>
+        <v>34.133031370000005</v>
+      </c>
+      <c r="E14" s="5">
+        <f>+SUM(E2:E13)</f>
+        <v>49.359305090000007</v>
+      </c>
+      <c r="F14" s="5">
+        <f>+SUM(F2:F13)</f>
+        <v>73.491345959761659</v>
+      </c>
+      <c r="G14" s="5">
+        <f>+SUM(G2:G13)</f>
+        <v>36.953714519999998</v>
+      </c>
+      <c r="H14" s="5">
+        <f>+SUM(H2:H13)</f>
+        <v>15.847577930230001</v>
+      </c>
+      <c r="I14" s="5">
+        <f>+SUM(I2:I13)</f>
+        <v>7.4808834300000004</v>
+      </c>
+      <c r="J14" s="5">
+        <f>+SUM(J2:J13)</f>
+        <v>4.0619130575</v>
+      </c>
+      <c r="K14" s="5">
+        <f>+SUM(K2:K13)</f>
+        <v>5.8828657</v>
+      </c>
+      <c r="L14" s="5">
+        <f>+SUM(L2:L13)</f>
+        <v>7.3869768860000002</v>
+      </c>
+      <c r="M14" s="5">
+        <f>+SUM(M2:M13)</f>
+        <v>24.362225892369995</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B16">
+        <f t="array" ref="B16:M16">TRANSPOSE(N2:N13)</f>
+        <v>83.492336422509979</v>
+      </c>
+      <c r="C16">
+        <v>90.879313784761649</v>
+      </c>
+      <c r="D16">
+        <v>34.133031362509982</v>
+      </c>
+      <c r="E16">
+        <v>49.359305059999997</v>
+      </c>
+      <c r="F16">
+        <v>73.464109063600006</v>
+      </c>
+      <c r="G16">
+        <v>36.953714519999998</v>
+      </c>
+      <c r="H16">
+        <v>15.874814386000001</v>
+      </c>
+      <c r="I16">
+        <v>7.4808834299999996</v>
+      </c>
+      <c r="J16">
+        <v>4.0619130575</v>
+      </c>
+      <c r="K16">
+        <v>5.8828657</v>
+      </c>
+      <c r="L16">
+        <v>7.3869768858900002</v>
+      </c>
+      <c r="M16">
+        <v>24.362225894000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B18" s="2">
+        <f>ROUND(B14-B16,1)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:M18" si="0">ROUND(C14-C16,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="5">
+        <v>12733.68651</v>
+      </c>
+      <c r="F20" s="7">
+        <f>+SUM(F3:F3)</f>
+        <v>56.02172243576166</v>
+      </c>
+      <c r="H20" s="7">
+        <f>+SUM(H3:H3)</f>
+        <v>10.495365456630001</v>
+      </c>
+      <c r="M20" s="7">
+        <f>+SUM(M3:M3)</f>
+        <v>24.362225892369995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A22" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="J22" s="7">
+        <f>+J6-C39</f>
+        <v>4.0619130575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="F23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="J23" s="7">
+        <f>+H10-C39</f>
+        <v>2.5385214375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B25">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="B31" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B42" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="5">
+        <v>3.1605375580000001</v>
+      </c>
+      <c r="D43" s="7" t="e">
+        <f>+#REF!-B47</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F43" s="7" t="e">
+        <f>+F3+D43</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="5">
+        <v>6.9137747879999996</v>
+      </c>
+      <c r="D44" s="7" t="e">
+        <f>+#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7" t="e">
+        <f>+#REF!+D44</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="5">
+        <v>4.4456911320000003</v>
+      </c>
+      <c r="D45" s="7" t="e">
+        <f>+#REF!-#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F45" s="7" t="e">
+        <f>+#REF!+D45</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B47" s="7">
+        <f>+SUM(B43:B45)</f>
+        <v>14.520003478</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B51" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="5">
+        <v>14.16830558289</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="5">
+        <v>0.17356569899999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B57" s="7">
+        <f>+SUM(B53:B55)</f>
+        <v>14.341871281889999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B59" s="7">
+        <v>1.8377085351100018</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="5">
+        <v>2.9878268870000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B62" s="7">
+        <f>+B60-B59</f>
+        <v>1.1501183518899984</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:N14">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:M18">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43:B45">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53:B55">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="notEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -3768,7 +4850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y58"/>
   <sheetViews>
@@ -5808,7 +6890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA39"/>
   <sheetViews>
@@ -7763,7 +8845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA177"/>
   <sheetViews>

</xml_diff>